<commit_message>
EPBDS-7689 Access to Condition parameters in another Condition expression Rules and Smart Rules (external conditions).
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7689_ExternalConditions_ConflictsResolving.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7689_ExternalConditions_ConflictsResolving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9105_ExternalConditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B1ECDE-B9FD-4B3B-873B-D3422B6FCF9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333D4313-0002-48F6-BA6B-4D0CE1B126CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3570" yWindow="345" windowWidth="21600" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>Inputs</t>
   </si>
@@ -78,21 +78,9 @@
     <t>InputObject  myObj</t>
   </si>
   <si>
-    <t>Integer param</t>
-  </si>
-  <si>
-    <t>new OutputObject(myObj.someInputText, param)</t>
-  </si>
-  <si>
     <t>Datatype OutputObject</t>
   </si>
   <si>
-    <t>Integer tra</t>
-  </si>
-  <si>
-    <t>System.out.println(tra)</t>
-  </si>
-  <si>
     <t>externalConditon2</t>
   </si>
   <si>
@@ -111,21 +99,12 @@
     <t>myObj.someInputNumber + d1</t>
   </si>
   <si>
-    <t>Integer _tra</t>
-  </si>
-  <si>
     <t>myObj.someInputNumber == tra + _tra</t>
   </si>
   <si>
-    <t>Integer Param</t>
-  </si>
-  <si>
     <t>Integer Tra</t>
   </si>
   <si>
-    <t>new OutputObject(myObj.someInputText, tra)</t>
-  </si>
-  <si>
     <t>Integer _Tra</t>
   </si>
   <si>
@@ -133,6 +112,24 @@
   </si>
   <si>
     <t>new OutputObject(myObj.someInputText, Tra)</t>
+  </si>
+  <si>
+    <t>externalConditon3</t>
+  </si>
+  <si>
+    <t>externalConditon4</t>
+  </si>
+  <si>
+    <t>Integer _Tra_1</t>
+  </si>
+  <si>
+    <t>myObj.someInputNumber == _tra_1 + _tra</t>
+  </si>
+  <si>
+    <t>SmartRules OutputObject mySmart2( InputObject x, String tra)</t>
+  </si>
+  <si>
+    <t>//SmartRules OutputObject mySmart2( InputObject x, String tra)</t>
   </si>
 </sst>
 </file>
@@ -540,25 +537,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C10:G46"/>
+  <dimension ref="C10:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="22.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -569,34 +569,48 @@
       <c r="F11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>3</v>
       </c>
@@ -604,13 +618,19 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>4</v>
       </c>
@@ -628,7 +648,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
@@ -636,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
@@ -674,13 +694,13 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F24" t="s">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
@@ -694,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
@@ -713,7 +733,7 @@
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
@@ -721,13 +741,19 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>5</v>
       </c>
@@ -735,10 +761,16 @@
         <v>5</v>
       </c>
       <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>6</v>
       </c>
@@ -746,10 +778,16 @@
         <v>6</v>
       </c>
       <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>7</v>
       </c>
@@ -757,15 +795,21 @@
         <v>7</v>
       </c>
       <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>7</v>
+      </c>
+      <c r="G35">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>10</v>
       </c>
@@ -773,7 +817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>11</v>
       </c>
@@ -781,12 +825,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>10</v>
       </c>
@@ -794,7 +838,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>11</v>
       </c>
@@ -802,10 +846,61 @@
         <v>15</v>
       </c>
     </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>